<commit_message>
Added new config yml and excel files
</commit_message>
<xml_diff>
--- a/samples/idaithalam-excel-apitesting/src/test/resources/virtualan_collection_pet_sheet_2.xlsx
+++ b/samples/idaithalam-excel-apitesting/src/test/resources/virtualan_collection_pet_sheet_2.xlsx
@@ -1,18 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dell\Desktop\Extra\November-28\idaithalam\samples\idaithalam-excel-apitesting\src\test\resources\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1DD365B-1A2B-4FED-8E2F-51B8BB7AF8AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <bookViews>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+  </bookViews>
   <sheets>
-    <sheet state="visible" name="API-Testing" sheetId="1" r:id="rId4"/>
-    <sheet state="visible" name="API-Testing-Sheet2" sheetId="2" r:id="rId5"/>
+    <sheet name="API-Testing" sheetId="1" r:id="rId1"/>
+    <sheet name="API-Testing-Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
-  <definedNames/>
-  <calcPr/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="49">
   <si>
     <t>TestCaseName</t>
   </si>
@@ -85,21 +94,21 @@
   <si>
     <r>
       <rPr>
+        <b/>
+        <u/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
         <rFont val="Inconsolata"/>
-        <b/>
-        <color rgb="FF000000"/>
-        <sz val="11.0"/>
-        <u/>
       </rPr>
       <t>tag=</t>
     </r>
     <r>
       <rPr>
+        <b/>
+        <u/>
+        <sz val="11"/>
+        <color rgb="FF1155CC"/>
         <rFont val="Inconsolata"/>
-        <b/>
-        <color rgb="FF1155CC"/>
-        <sz val="11.0"/>
-        <u/>
       </rPr>
       <t>grey</t>
     </r>
@@ -116,21 +125,21 @@
   <si>
     <r>
       <rPr>
+        <b/>
+        <u/>
+        <sz val="11"/>
+        <color rgb="FF1155CC"/>
         <rFont val="Inconsolata"/>
-        <b/>
-        <color rgb="FF1155CC"/>
-        <sz val="11.0"/>
-        <u/>
       </rPr>
       <t>https://live.virtualandemo.com/api/pets/findByTags?tags=</t>
     </r>
     <r>
       <rPr>
+        <b/>
+        <u/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
         <rFont val="Inconsolata"/>
-        <b/>
-        <color rgb="FF000000"/>
-        <sz val="11.0"/>
-        <u/>
       </rPr>
       <t>[tag]</t>
     </r>
@@ -180,49 +189,46 @@
   <si>
     <r>
       <rPr>
+        <b/>
+        <u/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
         <rFont val="Inconsolata"/>
-        <b/>
-        <color rgb="FF000000"/>
-        <sz val="11.0"/>
-        <u/>
       </rPr>
       <t>tag=</t>
     </r>
     <r>
       <rPr>
+        <b/>
+        <u/>
+        <sz val="11"/>
+        <color rgb="FF1155CC"/>
         <rFont val="Inconsolata"/>
-        <b/>
-        <color rgb="FF1155CC"/>
-        <sz val="11.0"/>
-        <u/>
       </rPr>
       <t>grey</t>
     </r>
   </si>
   <si>
-    <t>okta=http://www.okta.com/okta2</t>
-  </si>
-  <si>
     <t>PetGet_2</t>
   </si>
   <si>
     <r>
       <rPr>
+        <b/>
+        <u/>
+        <sz val="11"/>
+        <color rgb="FF1155CC"/>
         <rFont val="Inconsolata"/>
-        <b/>
-        <color rgb="FF1155CC"/>
-        <sz val="11.0"/>
-        <u/>
       </rPr>
       <t>https://live.virtualandemo.com/api/pets/findByTags?tags=</t>
     </r>
     <r>
       <rPr>
+        <b/>
+        <u/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
         <rFont val="Inconsolata"/>
-        <b/>
-        <color rgb="FF000000"/>
-        <sz val="11.0"/>
-        <u/>
       </rPr>
       <t>[tag]</t>
     </r>
@@ -235,50 +241,66 @@
   </si>
   <si>
     <t>PetPost_3-Test</t>
+  </si>
+  <si>
+    <t>ExcludeFields</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="8">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="9">
     <font>
-      <sz val="10.0"/>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
     </font>
     <font>
+      <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
     </font>
     <font>
       <b/>
+      <sz val="10"/>
       <color rgb="FF008000"/>
       <name val="Consolas"/>
     </font>
-    <font/>
     <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
     </font>
     <font>
       <u/>
-      <sz val="9.0"/>
+      <sz val="9"/>
       <color rgb="FF505050"/>
       <name val="Arial"/>
     </font>
     <font>
       <b/>
       <u/>
-      <sz val="11.0"/>
+      <sz val="11"/>
       <color rgb="FF1155CC"/>
       <name val="Docs-Inconsolata"/>
     </font>
     <font>
       <b/>
       <u/>
-      <sz val="11.0"/>
+      <sz val="11"/>
       <color rgb="FF1155CC"/>
+      <name val="Inconsolata"/>
+    </font>
+    <font>
+      <b/>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
       <name val="Inconsolata"/>
     </font>
   </fonts>
@@ -287,7 +309,7 @@
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="lightGray"/>
+      <patternFill patternType="gray125"/>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -297,65 +319,68 @@
     </fill>
   </fills>
   <borders count="1">
-    <border/>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="8">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
-    <xf borderId="0" fillId="2" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
-      <alignment readingOrder="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="2" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="2" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="2" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle xfId="0" name="Normal" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="1">
+  <dxfs count="2">
     <dxf>
-      <font/>
       <fill>
         <patternFill patternType="solid">
           <fgColor rgb="FFB7E1CD"/>
           <bgColor rgb="FFB7E1CD"/>
         </patternFill>
       </fill>
-      <border/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFB7E1CD"/>
+          <bgColor rgb="FFB7E1CD"/>
+        </patternFill>
+      </fill>
     </dxf>
   </dxfs>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
-<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheets">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Sheets">
   <a:themeElements>
     <a:clrScheme name="Sheets">
       <a:dk1>
@@ -545,27 +570,32 @@
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="A1:N4"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="I2" sqref="I2"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
-    <col customWidth="1" min="2" max="2" width="18.14"/>
-    <col customWidth="1" min="3" max="3" width="176.14"/>
-    <col customWidth="1" min="7" max="7" width="23.29"/>
-    <col customWidth="1" min="11" max="11" width="49.29"/>
-    <col customWidth="1" min="12" max="12" width="24.29"/>
+    <col min="2" max="2" width="18.109375" customWidth="1"/>
+    <col min="3" max="3" width="176.109375" customWidth="1"/>
+    <col min="7" max="7" width="23.33203125" customWidth="1"/>
+    <col min="11" max="11" width="49.33203125" customWidth="1"/>
+    <col min="12" max="12" width="24.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:14" ht="13.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -591,7 +621,7 @@
         <v>7</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>8</v>
+        <v>48</v>
       </c>
       <c r="J1" s="3" t="s">
         <v>9</v>
@@ -609,7 +639,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" spans="1:14" ht="15.75" customHeight="1">
       <c r="A2" s="4" t="s">
         <v>14</v>
       </c>
@@ -638,7 +668,7 @@
         <v>22</v>
       </c>
       <c r="J2" s="1">
-        <v>200.0</v>
+        <v>200</v>
       </c>
       <c r="L2" s="6" t="s">
         <v>23</v>
@@ -647,7 +677,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="3">
+    <row r="3" spans="1:14" ht="15.75" customHeight="1">
       <c r="A3" s="1" t="s">
         <v>25</v>
       </c>
@@ -667,7 +697,7 @@
         <v>30</v>
       </c>
       <c r="J3" s="1">
-        <v>200.0</v>
+        <v>200</v>
       </c>
       <c r="K3" s="1" t="s">
         <v>31</v>
@@ -676,7 +706,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="4">
+    <row r="4" spans="1:14" ht="15.75" customHeight="1">
       <c r="A4" s="1" t="s">
         <v>33</v>
       </c>
@@ -699,12 +729,227 @@
         <v>21</v>
       </c>
       <c r="J4" s="1">
-        <v>200.0</v>
+        <v>200</v>
       </c>
       <c r="L4" s="1" t="s">
         <v>38</v>
       </c>
       <c r="N4" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="F3">
+    <cfRule type="notContainsBlanks" dxfId="1" priority="1">
+      <formula>LEN(TRIM(F3))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <hyperlinks>
+    <hyperlink ref="C2" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="L2" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="C3" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
+    <hyperlink ref="C4" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <sheetPr>
+    <outlinePr summaryBelow="0" summaryRight="0"/>
+  </sheetPr>
+  <dimension ref="A1:N5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="M2" sqref="M2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1"/>
+  <cols>
+    <col min="2" max="2" width="18.109375" customWidth="1"/>
+    <col min="3" max="3" width="176.109375" customWidth="1"/>
+    <col min="7" max="7" width="23.33203125" customWidth="1"/>
+    <col min="11" max="11" width="49.33203125" customWidth="1"/>
+    <col min="12" max="12" width="24.33203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:14" ht="13.2">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="N1" s="3" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" ht="15.75" customHeight="1">
+      <c r="A2" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="J2" s="1">
+        <v>200</v>
+      </c>
+      <c r="L2" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="M2" s="1"/>
+      <c r="N2" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" ht="15.75" customHeight="1">
+      <c r="A3" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C3" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="J3" s="1">
+        <v>200</v>
+      </c>
+      <c r="K3" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="M3" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="N3" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" ht="15.75" customHeight="1">
+      <c r="A4" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C4" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="J4" s="1">
+        <v>200</v>
+      </c>
+      <c r="L4" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="N4" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" ht="15.75" customHeight="1">
+      <c r="A5" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C5" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="J5" s="1">
+        <v>200</v>
+      </c>
+      <c r="L5" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="N5" s="1" t="s">
         <v>32</v>
       </c>
     </row>
@@ -715,226 +960,12 @@
     </cfRule>
   </conditionalFormatting>
   <hyperlinks>
-    <hyperlink r:id="rId1" ref="C2"/>
-    <hyperlink r:id="rId2" ref="L2"/>
-    <hyperlink r:id="rId3" ref="C3"/>
-    <hyperlink r:id="rId4" ref="C4"/>
+    <hyperlink ref="C2" r:id="rId1" xr:uid="{00000000-0004-0000-0100-000000000000}"/>
+    <hyperlink ref="L2" r:id="rId2" xr:uid="{00000000-0004-0000-0100-000001000000}"/>
+    <hyperlink ref="C3" r:id="rId3" xr:uid="{00000000-0004-0000-0100-000002000000}"/>
+    <hyperlink ref="C4" r:id="rId4" xr:uid="{00000000-0004-0000-0100-000003000000}"/>
+    <hyperlink ref="C5" r:id="rId5" xr:uid="{00000000-0004-0000-0100-000004000000}"/>
   </hyperlinks>
-  <drawing r:id="rId5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="0" summaryRight="0"/>
-  </sheetPr>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
-  <cols>
-    <col customWidth="1" min="2" max="2" width="18.14"/>
-    <col customWidth="1" min="3" max="3" width="176.14"/>
-    <col customWidth="1" min="7" max="7" width="23.29"/>
-    <col customWidth="1" min="11" max="11" width="49.29"/>
-    <col customWidth="1" min="12" max="12" width="24.29"/>
-  </cols>
-  <sheetData>
-    <row r="1">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="J1" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="M1" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="N1" s="3" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="B2" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="C2" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="H2" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="I2" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="J2" s="1">
-        <v>200.0</v>
-      </c>
-      <c r="L2" s="6" t="s">
-        <v>42</v>
-      </c>
-      <c r="M2" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="N2" s="1" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="C3" s="7" t="s">
-        <v>45</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="H3" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="J3" s="1">
-        <v>200.0</v>
-      </c>
-      <c r="K3" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="M3" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="N3" s="1" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="C4" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="H4" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="J4" s="1">
-        <v>200.0</v>
-      </c>
-      <c r="L4" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="N4" s="1" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="C5" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="F5" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="H5" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="J5" s="1">
-        <v>200.0</v>
-      </c>
-      <c r="L5" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="N5" s="1" t="s">
-        <v>32</v>
-      </c>
-    </row>
-  </sheetData>
-  <conditionalFormatting sqref="F3">
-    <cfRule type="notContainsBlanks" dxfId="0" priority="1">
-      <formula>LEN(TRIM(F3))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <hyperlinks>
-    <hyperlink r:id="rId1" ref="C2"/>
-    <hyperlink r:id="rId2" ref="L2"/>
-    <hyperlink r:id="rId3" ref="C3"/>
-    <hyperlink r:id="rId4" ref="C4"/>
-    <hyperlink r:id="rId5" ref="C5"/>
-  </hyperlinks>
-  <drawing r:id="rId6"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>